<commit_message>
Update xlsx file with price > 1000
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -39,7 +39,7 @@
     <t>https://www.skroutz.gr/s/20060269/Apple-iPhone-11-64GB.html</t>
   </si>
   <si>
-    <t>900.00</t>
+    <t>1100.00</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>